<commit_message>
bijgewerkt voor tcs review
</commit_message>
<xml_diff>
--- a/IMKL2.x/3. extraregels/ExtraRegels-changelog.xlsx
+++ b/IMKL2.x/3. extraregels/ExtraRegels-changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjanssen\Documents\GitHub\imkl2015-review\IMKL2.x\3. extraregels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1D8124-2CFA-4AAA-9A3B-F6BA577A7CE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994C36B1-66F9-4696-82C3-06A4AD7D125F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{894B1FF5-8DFC-4651-A7C4-67B2EE5B0E46}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="66">
   <si>
     <t>Datum</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>Maximaal 1 algemene bijlage</t>
-  </si>
-  <si>
-    <t>Leidingelement</t>
   </si>
   <si>
     <t>rotatiehoekSymbool</t>
@@ -224,6 +221,18 @@
   </si>
   <si>
     <t>de cardinaliteit stond op 1 terwijl het model 1..* aangeeft. In de tabbladen is 1 op 1..* gezet maar met een constraint aangegeven dat het max 1 is.</t>
+  </si>
+  <si>
+    <t>Leidingelement (appurtenance)</t>
+  </si>
+  <si>
+    <t>AanduidingEisVoorzorgsmaatregel</t>
+  </si>
+  <si>
+    <t>geometrie</t>
+  </si>
+  <si>
+    <t>Geometrie is vlak of multivlak</t>
   </si>
 </sst>
 </file>
@@ -672,8 +681,8 @@
   <dimension ref="A1:J179"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -734,7 +743,7 @@
         <v>16</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" s="10">
         <v>269</v>
@@ -752,7 +761,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" s="10">
         <v>269</v>
@@ -770,7 +779,7 @@
         <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" s="10">
         <v>269</v>
@@ -788,7 +797,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="10">
         <v>269</v>
@@ -974,7 +983,7 @@
         <v>32</v>
       </c>
       <c r="E16" s="10">
-        <v>195</v>
+        <v>192.19499999999999</v>
       </c>
       <c r="F16" s="6"/>
       <c r="J16" s="11"/>
@@ -984,13 +993,13 @@
         <v>43973</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="E17" s="10">
         <v>282</v>
@@ -1003,13 +1012,13 @@
         <v>43973</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="E18" s="10">
         <v>239</v>
@@ -1025,10 +1034,10 @@
         <v>30</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="10">
         <v>214</v>
@@ -1041,10 +1050,10 @@
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E20" s="10">
         <v>214</v>
@@ -1059,10 +1068,10 @@
         <v>28</v>
       </c>
       <c r="C21" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="E21" s="10">
         <v>213</v>
@@ -1080,7 +1089,7 @@
         <v>11</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E22" s="10">
         <v>191</v>
@@ -1096,7 +1105,7 @@
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23" s="10">
         <v>190</v>
@@ -1108,16 +1117,16 @@
         <v>43973</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>48</v>
       </c>
       <c r="F24" s="6"/>
     </row>
@@ -1129,10 +1138,10 @@
         <v>31</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E25" s="10">
         <v>197</v>
@@ -1147,10 +1156,10 @@
         <v>31</v>
       </c>
       <c r="C26" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="E26" s="10">
         <v>197</v>
@@ -1162,13 +1171,13 @@
         <v>43973</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="E27" s="10">
         <v>193</v>
@@ -1180,13 +1189,13 @@
         <v>43973</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="E28" s="10">
         <v>286</v>
@@ -1198,23 +1207,33 @@
         <v>43992</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="10"/>
+      <c r="A30" s="6">
+        <v>44008</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="10">
+        <v>210</v>
+      </c>
       <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -2574,6 +2593,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003ADD3040E3157B4E913BCA65F34844D7" ma:contentTypeVersion="10" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c1765059aa1475931adc12138fdcfd8c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aafb19fa-82be-411d-a6df-c75e9235a4ea" xmlns:ns3="3dfebdfe-2b22-40ba-8672-9fbc9b4066c4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="42d79c55539af1f9f274032ce6041302" ns2:_="" ns3:_="">
     <xsd:import namespace="aafb19fa-82be-411d-a6df-c75e9235a4ea"/>
@@ -2776,22 +2810,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7893A73B-81F0-482A-B793-D93E5F8DCA71}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB1489CD-B12A-4704-A7E2-006D773FFFBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0C9FDDB-2830-4DD6-A847-D844746B12F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2808,21 +2844,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB1489CD-B12A-4704-A7E2-006D773FFFBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7893A73B-81F0-482A-B793-D93E5F8DCA71}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
klaargezet voor rc intern
</commit_message>
<xml_diff>
--- a/IMKL2.x/3. extraregels/ExtraRegels-changelog.xlsx
+++ b/IMKL2.x/3. extraregels/ExtraRegels-changelog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjanssen\Documents\GitHub\imkl2015-review\IMKL2.x\3. extraregels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A995385D-E00E-46C2-A849-B8B65B807F6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFBD265-DE18-4F81-8A4C-AD19F0780B27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18030" yWindow="-6390" windowWidth="14400" windowHeight="10755" xr2:uid="{894B1FF5-8DFC-4651-A7C4-67B2EE5B0E46}"/>
+    <workbookView xWindow="-19320" yWindow="-7680" windowWidth="19440" windowHeight="15000" xr2:uid="{894B1FF5-8DFC-4651-A7C4-67B2EE5B0E46}"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="129">
   <si>
     <t>Datum</t>
   </si>
@@ -438,6 +438,12 @@
   </si>
   <si>
     <t>Appurtenance</t>
+  </si>
+  <si>
+    <t>Alle</t>
+  </si>
+  <si>
+    <t>De rood, groen, grijs codering verwijderd. Alles is nu zwart</t>
   </si>
 </sst>
 </file>
@@ -499,7 +505,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -512,13 +518,34 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -527,15 +554,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -549,9 +573,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -560,9 +581,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -573,26 +591,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -913,2198 +964,2259 @@
   <dimension ref="A1:J182"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E77" sqref="C77:E77"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+      <c r="A2" s="18">
         <v>43959</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="20">
         <v>269</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+      <c r="A3" s="18">
         <v>43959</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="20">
         <v>269</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+      <c r="A4" s="18">
         <v>43959</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="20">
         <v>269</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+      <c r="A5" s="18">
         <v>43959</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="20">
         <v>269</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+      <c r="A6" s="18">
         <v>43959</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="20">
         <v>269</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+      <c r="A7" s="18">
         <v>43959</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="20">
         <v>269</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
+      <c r="A8" s="18">
         <v>43959</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="20">
         <v>269</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
+      <c r="A9" s="18">
         <v>43959</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="20">
         <v>269</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
+      <c r="A10" s="18">
         <v>43959</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="20">
         <v>269</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
+      <c r="A11" s="18">
         <v>43959</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="20">
         <v>269</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+      <c r="A12" s="18">
         <v>43959</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="20">
         <v>269</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
+      <c r="A13" s="18">
         <v>43959</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="20">
         <v>269</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="J13" s="11"/>
+      <c r="F13" s="18"/>
+      <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+      <c r="A14" s="18">
         <v>43959</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="20">
         <v>269</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="J14" s="11"/>
+      <c r="F14" s="19"/>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
+      <c r="A15" s="18">
         <v>43959</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="20">
         <v>269</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="J15" s="11"/>
+      <c r="F15" s="19"/>
+      <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
+      <c r="A16" s="18">
         <v>43959</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="20">
         <v>269</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="J16" s="11"/>
+      <c r="F16" s="19"/>
+      <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
+      <c r="A17" s="18">
         <v>43973</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="20">
         <v>192.19499999999999</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="J17" s="11"/>
+      <c r="F17" s="18"/>
+      <c r="J17" s="9"/>
     </row>
     <row r="18" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
+      <c r="A18" s="18">
         <v>43973</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="20">
         <v>282</v>
       </c>
-      <c r="F18" s="6"/>
-      <c r="J18" s="11"/>
+      <c r="F18" s="18"/>
+      <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
+      <c r="A19" s="18">
         <v>43973</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="20">
         <v>239</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="J19" s="12"/>
+      <c r="F19" s="19"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
+      <c r="A20" s="18">
         <v>43973</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="20">
         <v>214</v>
       </c>
-      <c r="F20" s="6"/>
+      <c r="F20" s="18"/>
     </row>
     <row r="21" spans="1:10" ht="24" x14ac:dyDescent="0.2">
-      <c r="A21" s="6">
+      <c r="A21" s="18">
         <v>43973</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="20">
         <v>214</v>
       </c>
-      <c r="F21" s="6"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
+      <c r="A22" s="18">
         <v>43973</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="20">
         <v>213</v>
       </c>
-      <c r="F22" s="6"/>
+      <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:10" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6">
+      <c r="A23" s="18">
         <v>43973</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="20">
         <v>191</v>
       </c>
-      <c r="F23" s="6"/>
+      <c r="F23" s="18"/>
     </row>
     <row r="24" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A24" s="6">
+      <c r="A24" s="18">
         <v>43973</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6" t="s">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="20">
         <v>190</v>
       </c>
-      <c r="F24" s="6"/>
+      <c r="F24" s="18"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="6">
+      <c r="A25" s="18">
         <v>43973</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="6"/>
+      <c r="F25" s="18"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="6">
+      <c r="A26" s="18">
         <v>43973</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="20">
         <v>197</v>
       </c>
-      <c r="F26" s="6"/>
+      <c r="F26" s="18"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="6">
+      <c r="A27" s="18">
         <v>43973</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="20">
         <v>197</v>
       </c>
-      <c r="F27" s="6"/>
+      <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="6">
+      <c r="A28" s="18">
         <v>43973</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="20">
         <v>193</v>
       </c>
-      <c r="F28" s="6"/>
+      <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="6">
+      <c r="A29" s="18">
         <v>43973</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="20">
         <v>286</v>
       </c>
-      <c r="F29" s="6"/>
+      <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:10" ht="36" x14ac:dyDescent="0.2">
-      <c r="A30" s="6">
+      <c r="A30" s="18">
         <v>43992</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="6"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="6">
+      <c r="A31" s="18">
         <v>44008</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="20">
         <v>210</v>
       </c>
-      <c r="F31" s="6"/>
+      <c r="F31" s="18"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="6">
+      <c r="A32" s="18">
         <v>44018</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="20">
         <v>219</v>
       </c>
-      <c r="F32" s="5"/>
+      <c r="F32" s="19"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="6">
+      <c r="A33" s="18">
         <v>44018</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="5"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="19"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="6">
+      <c r="A34" s="18">
         <v>44018</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="5"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="19"/>
     </row>
     <row r="35" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="6">
+      <c r="A35" s="18">
         <v>44018</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="5"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="19"/>
     </row>
     <row r="36" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="6">
+      <c r="A36" s="18">
         <v>44018</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="5"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="19"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="6">
+      <c r="A37" s="18">
         <v>44018</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="5"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="19"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="6">
+      <c r="A38" s="18">
         <v>44018</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="10"/>
-      <c r="F38" s="5"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="19"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="6">
+      <c r="A39" s="18">
         <v>44018</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="10"/>
-      <c r="F39" s="6"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="18"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="6">
+      <c r="A40" s="18">
         <v>44018</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E40" s="10"/>
-      <c r="F40" s="6"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="18"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="6">
+      <c r="A41" s="18">
         <v>44018</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6" t="s">
+      <c r="C41" s="18"/>
+      <c r="D41" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E41" s="20">
         <v>240</v>
       </c>
-      <c r="F41" s="5"/>
+      <c r="F41" s="19"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="6">
+      <c r="A42" s="18">
         <v>44018</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6" t="s">
+      <c r="C42" s="18"/>
+      <c r="D42" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E42" s="10"/>
-      <c r="F42" s="5"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="19"/>
     </row>
     <row r="43" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="6">
+      <c r="A43" s="18">
         <v>44018</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6" t="s">
+      <c r="C43" s="18"/>
+      <c r="D43" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E43" s="10"/>
-      <c r="F43" s="5"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="19"/>
     </row>
     <row r="44" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="6">
+      <c r="A44" s="18">
         <v>44018</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="C44" s="17" t="s">
+      <c r="C44" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="20">
         <v>199</v>
       </c>
-      <c r="F44" s="5"/>
+      <c r="F44" s="19"/>
     </row>
     <row r="45" spans="1:6" ht="24" x14ac:dyDescent="0.2">
-      <c r="A45" s="6">
+      <c r="A45" s="18">
         <v>44018</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45" s="20">
         <v>199</v>
       </c>
-      <c r="F45" s="5"/>
-    </row>
-    <row r="46" spans="1:6" s="23" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="20">
+      <c r="F45" s="19"/>
+    </row>
+    <row r="46" spans="1:6" s="15" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="23">
         <v>44018</v>
       </c>
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D46" s="20" t="s">
+      <c r="D46" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="E46" s="22">
+      <c r="E46" s="25">
         <v>199</v>
       </c>
-      <c r="F46" s="23" t="s">
+      <c r="F46" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="23" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A47" s="20">
+    <row r="47" spans="1:6" s="15" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A47" s="23">
         <v>44018</v>
       </c>
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="D47" s="20" t="s">
+      <c r="D47" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="E47" s="22">
+      <c r="E47" s="25">
         <v>199</v>
       </c>
-      <c r="F47" s="23" t="s">
+      <c r="F47" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A48" s="6">
+    <row r="48" spans="1:6" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A48" s="18">
         <v>44018</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6" t="s">
+      <c r="C48" s="18"/>
+      <c r="D48" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="19"/>
-    </row>
-    <row r="49" spans="1:8" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A49" s="6">
+      <c r="E48" s="27"/>
+      <c r="F48" s="28"/>
+    </row>
+    <row r="49" spans="1:8" s="14" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A49" s="18">
         <v>44018</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6" t="s">
+      <c r="C49" s="18"/>
+      <c r="D49" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E49" s="19"/>
-    </row>
-    <row r="50" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="6">
+      <c r="E49" s="27"/>
+      <c r="F49" s="28"/>
+    </row>
+    <row r="50" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="18">
         <v>44018</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="D50" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E50" s="19">
+      <c r="E50" s="27">
         <v>296</v>
       </c>
+      <c r="F50" s="28"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="6">
+      <c r="A51" s="29">
         <v>44090</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6" t="s">
+      <c r="C51" s="29"/>
+      <c r="D51" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="E51" s="10"/>
-      <c r="F51" s="5"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="19"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6" t="s">
+      <c r="A52" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B52" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6" t="s">
+      <c r="C52" s="29"/>
+      <c r="D52" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="E52" s="10"/>
-      <c r="F52" s="5"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="19"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6" t="s">
+      <c r="A53" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B53" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D53" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="E53" s="10"/>
-      <c r="F53" s="5"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="19"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6" t="s">
+      <c r="A54" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B54" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D54" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="E54" s="10"/>
-      <c r="F54" s="5"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="19"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6" t="s">
+      <c r="A55" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B55" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D55" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="E55" s="10"/>
-      <c r="F55" s="5"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="19"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6" t="s">
+      <c r="A56" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B56" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6" t="s">
+      <c r="C56" s="29"/>
+      <c r="D56" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="E56" s="10"/>
-      <c r="F56" s="5"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="19"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="6"/>
-      <c r="B57" s="6" t="s">
+      <c r="A57" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B57" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="E57" s="10"/>
-      <c r="F57" s="5"/>
+      <c r="E57" s="30"/>
+      <c r="F57" s="19"/>
     </row>
     <row r="58" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6" t="s">
+      <c r="A58" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B58" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6" t="s">
+      <c r="C58" s="29"/>
+      <c r="D58" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="E58" s="10"/>
-      <c r="F58" s="5"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="19"/>
     </row>
     <row r="59" spans="1:8" ht="36" x14ac:dyDescent="0.2">
-      <c r="A59" s="6"/>
-      <c r="B59" s="6" t="s">
+      <c r="A59" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B59" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="E59" s="10"/>
-      <c r="F59" s="5"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="19"/>
     </row>
     <row r="60" spans="1:8" ht="24" x14ac:dyDescent="0.2">
-      <c r="A60" s="6"/>
-      <c r="B60" s="6" t="s">
+      <c r="A60" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B60" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="E60" s="10"/>
-      <c r="F60" s="5"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="19"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="6"/>
-      <c r="B61" s="6" t="s">
+      <c r="A61" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B61" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="D61" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="E61" s="10"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
+      <c r="E61" s="30"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6" t="s">
+      <c r="A62" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B62" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D62" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="E62" s="10"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="12"/>
-      <c r="H62" s="12"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="6"/>
-      <c r="B63" s="6" t="s">
+      <c r="A63" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B63" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D63" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="E63" s="10"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="6"/>
-      <c r="B64" s="6" t="s">
+      <c r="A64" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B64" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="D64" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="E64" s="10"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="6"/>
-      <c r="B65" s="6" t="s">
+      <c r="A65" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B65" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C65" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="D65" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="E65" s="10"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
+      <c r="E65" s="30"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="6"/>
-      <c r="B66" s="6" t="s">
+      <c r="A66" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B66" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="E66" s="10"/>
-      <c r="F66" s="6"/>
-      <c r="G66" s="12"/>
-      <c r="H66" s="12"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="6"/>
-      <c r="B67" s="6" t="s">
+      <c r="A67" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B67" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C67" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="D67" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="E67" s="10"/>
-      <c r="F67" s="6"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="12"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="6"/>
-      <c r="B68" s="6" t="s">
+      <c r="A68" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B68" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C68" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="D68" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="E68" s="10"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="12"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6" t="s">
+      <c r="A69" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B69" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C69" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="D69" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="E69" s="10"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="12"/>
-      <c r="H69" s="12"/>
+      <c r="E69" s="30"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="6"/>
-      <c r="B70" s="5" t="s">
+      <c r="A70" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B70" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="D70" s="6" t="s">
+      <c r="D70" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="E70" s="10"/>
-      <c r="F70" s="6"/>
-      <c r="G70" s="12"/>
-      <c r="H70" s="12"/>
+      <c r="E70" s="30"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="6"/>
-      <c r="B71" s="5" t="s">
+      <c r="A71" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B71" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C71" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="D71" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="E71" s="10"/>
-      <c r="F71" s="6"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="12"/>
+      <c r="E71" s="30"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="6"/>
-      <c r="B72" s="5" t="s">
+      <c r="A72" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B72" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5" t="s">
+      <c r="C72" s="31"/>
+      <c r="D72" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="E72" s="10"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="12"/>
+      <c r="E72" s="30"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="6"/>
-      <c r="B73" s="5" t="s">
+      <c r="A73" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B73" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5" t="s">
+      <c r="C73" s="31"/>
+      <c r="D73" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="E73" s="10"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="12"/>
-      <c r="H73" s="12"/>
+      <c r="E73" s="30"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="6"/>
-      <c r="B74" s="5" t="s">
+      <c r="A74" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B74" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C74" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="E74" s="10">
+      <c r="E74" s="30">
         <v>304</v>
       </c>
-      <c r="F74" s="5"/>
-      <c r="G74" s="12"/>
-      <c r="H74" s="12"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="6"/>
-      <c r="B75" s="5" t="s">
+      <c r="A75" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B75" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C75" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="E75" s="10">
+      <c r="E75" s="30">
         <v>304</v>
       </c>
-      <c r="F75" s="5"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="12"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="6"/>
-      <c r="B76" s="5" t="s">
+      <c r="A76" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B76" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C76" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="E76" s="10">
+      <c r="E76" s="30">
         <v>304</v>
       </c>
-      <c r="F76" s="5"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="12"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="10"/>
+      <c r="H76" s="10"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="6"/>
-      <c r="B77" s="5" t="s">
+      <c r="A77" s="29">
+        <v>44090</v>
+      </c>
+      <c r="B77" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="E77" s="10">
+      <c r="E77" s="30">
         <v>304</v>
       </c>
-      <c r="F77" s="5"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="12"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="6"/>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="12"/>
+      <c r="A78" s="29">
+        <v>44097</v>
+      </c>
+      <c r="B78" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C78" s="31"/>
+      <c r="D78" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="E78" s="30"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="6"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="10"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="12"/>
+      <c r="A79" s="5"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="6"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="10"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="12"/>
+      <c r="A80" s="5"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="10"/>
+      <c r="H80" s="10"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="6"/>
-      <c r="B81" s="5"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="10"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="12"/>
+      <c r="A81" s="5"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="10"/>
+      <c r="H81" s="10"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="6"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="10"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="12"/>
-      <c r="H82" s="12"/>
+      <c r="A82" s="5"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="10"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="6"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="10"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="12"/>
+      <c r="A83" s="5"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="10"/>
+      <c r="H83" s="10"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="6"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="10"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="12"/>
+      <c r="A84" s="5"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="10"/>
+      <c r="H84" s="10"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="6"/>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="10"/>
-      <c r="F85" s="5"/>
-      <c r="G85" s="12"/>
-      <c r="H85" s="12"/>
+      <c r="A85" s="5"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="10"/>
+      <c r="H85" s="10"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="6"/>
-      <c r="B86" s="5"/>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="10"/>
-      <c r="F86" s="5"/>
-      <c r="G86" s="12"/>
-      <c r="H86" s="12"/>
+      <c r="A86" s="5"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="10"/>
+      <c r="H86" s="10"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="6"/>
-      <c r="B87" s="5"/>
-      <c r="C87" s="5"/>
-      <c r="D87" s="5"/>
-      <c r="E87" s="10"/>
-      <c r="F87" s="5"/>
-      <c r="G87" s="12"/>
-      <c r="H87" s="12"/>
+      <c r="A87" s="5"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="10"/>
+      <c r="H87" s="10"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="6"/>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5"/>
-      <c r="D88" s="5"/>
-      <c r="E88" s="10"/>
-      <c r="F88" s="5"/>
-      <c r="G88" s="12"/>
-      <c r="H88" s="12"/>
+      <c r="A88" s="5"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="10"/>
+      <c r="H88" s="10"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="6"/>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="10"/>
-      <c r="F89" s="6"/>
-      <c r="G89" s="12"/>
-      <c r="H89" s="12"/>
+      <c r="A89" s="5"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="10"/>
+      <c r="H89" s="10"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" s="6"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="6"/>
-      <c r="G90" s="12"/>
-      <c r="H90" s="12"/>
+      <c r="A90" s="5"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="8"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="6"/>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="10"/>
-      <c r="F91" s="6"/>
-      <c r="G91" s="12"/>
-      <c r="H91" s="12"/>
+      <c r="A91" s="5"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="6"/>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="10"/>
-      <c r="F92" s="6"/>
-      <c r="G92" s="12"/>
-      <c r="H92" s="12"/>
+      <c r="A92" s="5"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="8"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="10"/>
+      <c r="H92" s="10"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="6"/>
-      <c r="B93" s="5"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="10"/>
-      <c r="F93" s="6"/>
-      <c r="G93" s="12"/>
-      <c r="H93" s="12"/>
+      <c r="A93" s="5"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="10"/>
+      <c r="H93" s="10"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="6"/>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="10"/>
-      <c r="F94" s="6"/>
-      <c r="G94" s="12"/>
-      <c r="H94" s="12"/>
+      <c r="A94" s="5"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="10"/>
+      <c r="H94" s="10"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="6"/>
-      <c r="B95" s="5"/>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="10"/>
-      <c r="F95" s="5"/>
-      <c r="G95" s="12"/>
-      <c r="H95" s="12"/>
+      <c r="A95" s="5"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="8"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="10"/>
+      <c r="H95" s="10"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="6"/>
-      <c r="B96" s="5"/>
-      <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="10"/>
-      <c r="F96" s="5"/>
-      <c r="G96" s="12"/>
-      <c r="H96" s="12"/>
+      <c r="A96" s="5"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="8"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="10"/>
+      <c r="H96" s="10"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="6"/>
-      <c r="B97" s="5"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="10"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="12"/>
-      <c r="H97" s="12"/>
+      <c r="A97" s="5"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="8"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="10"/>
+      <c r="H97" s="10"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="6"/>
-      <c r="B98" s="5"/>
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="10"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="12"/>
-      <c r="H98" s="12"/>
+      <c r="A98" s="5"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="8"/>
+      <c r="F98" s="4"/>
+      <c r="G98" s="10"/>
+      <c r="H98" s="10"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="6"/>
-      <c r="B99" s="5"/>
-      <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
-      <c r="E99" s="10"/>
-      <c r="F99" s="5"/>
-      <c r="G99" s="12"/>
-      <c r="H99" s="12"/>
+      <c r="A99" s="5"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="4"/>
+      <c r="G99" s="10"/>
+      <c r="H99" s="10"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="6"/>
-      <c r="B100" s="5"/>
-      <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="10"/>
-      <c r="F100" s="5"/>
-      <c r="G100" s="12"/>
-      <c r="H100" s="12"/>
+      <c r="A100" s="5"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="4"/>
+      <c r="G100" s="10"/>
+      <c r="H100" s="10"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="6"/>
-      <c r="B101" s="5"/>
-      <c r="C101" s="5"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="10"/>
-      <c r="F101" s="5"/>
-      <c r="G101" s="12"/>
-      <c r="H101" s="12"/>
+      <c r="A101" s="5"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="10"/>
+      <c r="H101" s="10"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="6"/>
-      <c r="B102" s="5"/>
-      <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="10"/>
-      <c r="F102" s="5"/>
-      <c r="G102" s="12"/>
-      <c r="H102" s="12"/>
+      <c r="A102" s="5"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="8"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="10"/>
+      <c r="H102" s="10"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="6"/>
-      <c r="B103" s="5"/>
-      <c r="C103" s="5"/>
-      <c r="D103" s="5"/>
-      <c r="E103" s="10"/>
-      <c r="F103" s="5"/>
-      <c r="G103" s="12"/>
-      <c r="H103" s="12"/>
+      <c r="A103" s="5"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="8"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="10"/>
+      <c r="H103" s="10"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="6"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="10"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="12"/>
-      <c r="H104" s="12"/>
+      <c r="A104" s="5"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="8"/>
+      <c r="F104" s="4"/>
+      <c r="G104" s="10"/>
+      <c r="H104" s="10"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="6"/>
-      <c r="B105" s="5"/>
-      <c r="C105" s="5"/>
-      <c r="D105" s="5"/>
-      <c r="E105" s="10"/>
-      <c r="F105" s="5"/>
-      <c r="G105" s="12"/>
-      <c r="H105" s="12"/>
+      <c r="A105" s="5"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="8"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="10"/>
+      <c r="H105" s="10"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="6"/>
-      <c r="B106" s="5"/>
-      <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
-      <c r="E106" s="10"/>
-      <c r="F106" s="5"/>
-      <c r="G106" s="12"/>
-      <c r="H106" s="12"/>
+      <c r="A106" s="5"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="4"/>
+      <c r="D106" s="4"/>
+      <c r="E106" s="8"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="10"/>
+      <c r="H106" s="10"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="6"/>
-      <c r="B107" s="5"/>
-      <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
-      <c r="E107" s="10"/>
-      <c r="F107" s="5"/>
+      <c r="A107" s="5"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="8"/>
+      <c r="F107" s="4"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="6"/>
-      <c r="B108" s="5"/>
-      <c r="C108" s="5"/>
-      <c r="D108" s="5"/>
-      <c r="E108" s="10"/>
-      <c r="F108" s="5"/>
+      <c r="A108" s="5"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="4"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="6"/>
-      <c r="B109" s="5"/>
-      <c r="C109" s="5"/>
-      <c r="D109" s="5"/>
-      <c r="E109" s="10"/>
-      <c r="F109" s="5"/>
+      <c r="A109" s="5"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="8"/>
+      <c r="F109" s="4"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="6"/>
-      <c r="B110" s="5"/>
-      <c r="C110" s="5"/>
-      <c r="D110" s="5"/>
-      <c r="E110" s="10"/>
-      <c r="F110" s="5"/>
+      <c r="A110" s="5"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" s="8"/>
+      <c r="F110" s="4"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A111" s="6"/>
-      <c r="B111" s="5"/>
-      <c r="C111" s="5"/>
-      <c r="D111" s="5"/>
-      <c r="E111" s="10"/>
-      <c r="F111" s="5"/>
+      <c r="A111" s="5"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="8"/>
+      <c r="F111" s="4"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="6"/>
-      <c r="B112" s="5"/>
-      <c r="C112" s="5"/>
-      <c r="D112" s="5"/>
-      <c r="E112" s="10"/>
-      <c r="F112" s="5"/>
+      <c r="A112" s="5"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="8"/>
+      <c r="F112" s="4"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113" s="6"/>
-      <c r="B113" s="5"/>
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="10"/>
-      <c r="F113" s="5"/>
+      <c r="A113" s="5"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="8"/>
+      <c r="F113" s="4"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A114" s="6"/>
-      <c r="B114" s="5"/>
-      <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
-      <c r="E114" s="10"/>
-      <c r="F114" s="5"/>
+      <c r="A114" s="5"/>
+      <c r="B114" s="4"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="8"/>
+      <c r="F114" s="4"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A115" s="6"/>
-      <c r="B115" s="5"/>
-      <c r="C115" s="5"/>
-      <c r="D115" s="5"/>
-      <c r="E115" s="10"/>
-      <c r="F115" s="5"/>
+      <c r="A115" s="5"/>
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="8"/>
+      <c r="F115" s="4"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A116" s="6"/>
-      <c r="B116" s="5"/>
-      <c r="C116" s="5"/>
-      <c r="D116" s="5"/>
-      <c r="E116" s="10"/>
-      <c r="F116" s="5"/>
+      <c r="A116" s="5"/>
+      <c r="B116" s="4"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
+      <c r="E116" s="8"/>
+      <c r="F116" s="4"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117" s="6"/>
-      <c r="B117" s="5"/>
-      <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
-      <c r="E117" s="10"/>
-      <c r="F117" s="5"/>
+      <c r="A117" s="5"/>
+      <c r="B117" s="4"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
+      <c r="E117" s="8"/>
+      <c r="F117" s="4"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118" s="6"/>
-      <c r="B118" s="5"/>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="10"/>
-      <c r="F118" s="5"/>
+      <c r="A118" s="5"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="8"/>
+      <c r="F118" s="4"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A119" s="6"/>
-      <c r="B119" s="5"/>
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
-      <c r="E119" s="10"/>
-      <c r="F119" s="5"/>
+      <c r="A119" s="5"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="8"/>
+      <c r="F119" s="4"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A120" s="6"/>
-      <c r="B120" s="5"/>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
-      <c r="E120" s="10"/>
-      <c r="F120" s="5"/>
+      <c r="A120" s="5"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="4"/>
+      <c r="E120" s="8"/>
+      <c r="F120" s="4"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121" s="6"/>
-      <c r="B121" s="5"/>
-      <c r="C121" s="5"/>
-      <c r="D121" s="5"/>
-      <c r="E121" s="10"/>
-      <c r="F121" s="5"/>
+      <c r="A121" s="5"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="8"/>
+      <c r="F121" s="4"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A122" s="6"/>
-      <c r="B122" s="5"/>
-      <c r="C122" s="5"/>
-      <c r="D122" s="5"/>
-      <c r="E122" s="10"/>
-      <c r="F122" s="5"/>
+      <c r="A122" s="5"/>
+      <c r="B122" s="4"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="8"/>
+      <c r="F122" s="4"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A123" s="6"/>
-      <c r="B123" s="5"/>
-      <c r="C123" s="5"/>
-      <c r="D123" s="5"/>
-      <c r="E123" s="10"/>
-      <c r="F123" s="5"/>
+      <c r="A123" s="5"/>
+      <c r="B123" s="4"/>
+      <c r="C123" s="4"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="8"/>
+      <c r="F123" s="4"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A124" s="6"/>
-      <c r="B124" s="6"/>
-      <c r="C124" s="5"/>
-      <c r="D124" s="5"/>
-      <c r="E124" s="10"/>
-      <c r="F124" s="5"/>
+      <c r="A124" s="5"/>
+      <c r="B124" s="5"/>
+      <c r="C124" s="4"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="8"/>
+      <c r="F124" s="4"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A125" s="6"/>
-      <c r="B125" s="5"/>
-      <c r="C125" s="5"/>
-      <c r="D125" s="5"/>
-      <c r="E125" s="10"/>
-      <c r="F125" s="5"/>
+      <c r="A125" s="5"/>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="8"/>
+      <c r="F125" s="4"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A126" s="6"/>
-      <c r="B126" s="5"/>
-      <c r="C126" s="5"/>
-      <c r="D126" s="5"/>
-      <c r="E126" s="10"/>
-      <c r="F126" s="5"/>
+      <c r="A126" s="5"/>
+      <c r="B126" s="4"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="8"/>
+      <c r="F126" s="4"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A127" s="6"/>
-      <c r="B127" s="5"/>
-      <c r="C127" s="5"/>
-      <c r="D127" s="5"/>
-      <c r="E127" s="10"/>
-      <c r="F127" s="5"/>
+      <c r="A127" s="5"/>
+      <c r="B127" s="4"/>
+      <c r="C127" s="4"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="8"/>
+      <c r="F127" s="4"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A128" s="6"/>
-      <c r="B128" s="6"/>
-      <c r="C128" s="6"/>
-      <c r="D128" s="6"/>
-      <c r="E128" s="10"/>
-      <c r="F128" s="6"/>
+      <c r="A128" s="5"/>
+      <c r="B128" s="5"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="8"/>
+      <c r="F128" s="5"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A129" s="6"/>
-      <c r="B129" s="6"/>
-      <c r="C129" s="6"/>
-      <c r="D129" s="6"/>
-      <c r="E129" s="10"/>
-      <c r="F129" s="6"/>
+      <c r="A129" s="5"/>
+      <c r="B129" s="5"/>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="8"/>
+      <c r="F129" s="5"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A130" s="6"/>
-      <c r="B130" s="6"/>
-      <c r="C130" s="6"/>
-      <c r="D130" s="6"/>
-      <c r="E130" s="10"/>
-      <c r="F130" s="6"/>
+      <c r="A130" s="5"/>
+      <c r="B130" s="5"/>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="8"/>
+      <c r="F130" s="5"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A131" s="14"/>
-      <c r="B131" s="7"/>
-      <c r="C131" s="7"/>
-      <c r="D131" s="7"/>
-      <c r="E131" s="10"/>
-      <c r="F131" s="7"/>
+      <c r="A131" s="11"/>
+      <c r="B131" s="6"/>
+      <c r="C131" s="6"/>
+      <c r="D131" s="6"/>
+      <c r="E131" s="8"/>
+      <c r="F131" s="6"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A132" s="14"/>
-      <c r="B132" s="7"/>
-      <c r="C132" s="7"/>
-      <c r="D132" s="7"/>
-      <c r="E132" s="10"/>
-      <c r="F132" s="7"/>
+      <c r="A132" s="11"/>
+      <c r="B132" s="6"/>
+      <c r="C132" s="6"/>
+      <c r="D132" s="6"/>
+      <c r="E132" s="8"/>
+      <c r="F132" s="6"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A133" s="14"/>
-      <c r="B133" s="7"/>
-      <c r="C133" s="7"/>
-      <c r="D133" s="7"/>
-      <c r="E133" s="10"/>
-      <c r="F133" s="7"/>
+      <c r="A133" s="11"/>
+      <c r="B133" s="6"/>
+      <c r="C133" s="6"/>
+      <c r="D133" s="6"/>
+      <c r="E133" s="8"/>
+      <c r="F133" s="6"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A134" s="14"/>
-      <c r="B134" s="7"/>
-      <c r="C134" s="7"/>
-      <c r="D134" s="7"/>
-      <c r="E134" s="10"/>
-      <c r="F134" s="7"/>
+      <c r="A134" s="11"/>
+      <c r="B134" s="6"/>
+      <c r="C134" s="6"/>
+      <c r="D134" s="6"/>
+      <c r="E134" s="8"/>
+      <c r="F134" s="6"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A135" s="14"/>
-      <c r="B135" s="7"/>
-      <c r="C135" s="7"/>
-      <c r="D135" s="7"/>
-      <c r="E135" s="10"/>
-      <c r="F135" s="7"/>
+      <c r="A135" s="11"/>
+      <c r="B135" s="6"/>
+      <c r="C135" s="6"/>
+      <c r="D135" s="6"/>
+      <c r="E135" s="8"/>
+      <c r="F135" s="6"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A136" s="14"/>
-      <c r="B136" s="7"/>
-      <c r="C136" s="7"/>
-      <c r="D136" s="7"/>
-      <c r="E136" s="10"/>
-      <c r="F136" s="7"/>
+      <c r="A136" s="11"/>
+      <c r="B136" s="6"/>
+      <c r="C136" s="6"/>
+      <c r="D136" s="6"/>
+      <c r="E136" s="8"/>
+      <c r="F136" s="6"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A137" s="14"/>
-      <c r="B137" s="7"/>
-      <c r="C137" s="7"/>
-      <c r="D137" s="7"/>
-      <c r="E137" s="10"/>
-      <c r="F137" s="7"/>
+      <c r="A137" s="11"/>
+      <c r="B137" s="6"/>
+      <c r="C137" s="6"/>
+      <c r="D137" s="6"/>
+      <c r="E137" s="8"/>
+      <c r="F137" s="6"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A138" s="14"/>
-      <c r="B138" s="7"/>
-      <c r="C138" s="7"/>
-      <c r="D138" s="7"/>
-      <c r="E138" s="10"/>
-      <c r="F138" s="7"/>
+      <c r="A138" s="11"/>
+      <c r="B138" s="6"/>
+      <c r="C138" s="6"/>
+      <c r="D138" s="6"/>
+      <c r="E138" s="8"/>
+      <c r="F138" s="6"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A139" s="7"/>
-      <c r="B139" s="7"/>
-      <c r="C139" s="7"/>
-      <c r="D139" s="7"/>
-      <c r="E139" s="15"/>
-      <c r="F139" s="7"/>
+      <c r="A139" s="6"/>
+      <c r="B139" s="6"/>
+      <c r="C139" s="6"/>
+      <c r="D139" s="6"/>
+      <c r="E139" s="12"/>
+      <c r="F139" s="6"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A140" s="7"/>
-      <c r="B140" s="7"/>
-      <c r="C140" s="7"/>
-      <c r="D140" s="7"/>
-      <c r="E140" s="15"/>
-      <c r="F140" s="7"/>
+      <c r="A140" s="6"/>
+      <c r="B140" s="6"/>
+      <c r="C140" s="6"/>
+      <c r="D140" s="6"/>
+      <c r="E140" s="12"/>
+      <c r="F140" s="6"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A141" s="7"/>
-      <c r="B141" s="7"/>
-      <c r="C141" s="7"/>
-      <c r="D141" s="7"/>
-      <c r="E141" s="15"/>
-      <c r="F141" s="7"/>
+      <c r="A141" s="6"/>
+      <c r="B141" s="6"/>
+      <c r="C141" s="6"/>
+      <c r="D141" s="6"/>
+      <c r="E141" s="12"/>
+      <c r="F141" s="6"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A142" s="7"/>
-      <c r="B142" s="7"/>
-      <c r="C142" s="7"/>
-      <c r="D142" s="7"/>
-      <c r="E142" s="15"/>
-      <c r="F142" s="7"/>
+      <c r="A142" s="6"/>
+      <c r="B142" s="6"/>
+      <c r="C142" s="6"/>
+      <c r="D142" s="6"/>
+      <c r="E142" s="12"/>
+      <c r="F142" s="6"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A143" s="7"/>
-      <c r="B143" s="7"/>
-      <c r="C143" s="7"/>
-      <c r="D143" s="7"/>
-      <c r="E143" s="15"/>
-      <c r="F143" s="7"/>
+      <c r="A143" s="6"/>
+      <c r="B143" s="6"/>
+      <c r="C143" s="6"/>
+      <c r="D143" s="6"/>
+      <c r="E143" s="12"/>
+      <c r="F143" s="6"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A144" s="7"/>
-      <c r="B144" s="7"/>
-      <c r="C144" s="7"/>
-      <c r="D144" s="7"/>
-      <c r="E144" s="15"/>
-      <c r="F144" s="7"/>
+      <c r="A144" s="6"/>
+      <c r="B144" s="6"/>
+      <c r="C144" s="6"/>
+      <c r="D144" s="6"/>
+      <c r="E144" s="12"/>
+      <c r="F144" s="6"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A145" s="7"/>
-      <c r="B145" s="7"/>
-      <c r="C145" s="7"/>
-      <c r="D145" s="7"/>
-      <c r="E145" s="15"/>
-      <c r="F145" s="7"/>
+      <c r="A145" s="6"/>
+      <c r="B145" s="6"/>
+      <c r="C145" s="6"/>
+      <c r="D145" s="6"/>
+      <c r="E145" s="12"/>
+      <c r="F145" s="6"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A146" s="7"/>
-      <c r="B146" s="7"/>
-      <c r="C146" s="7"/>
-      <c r="D146" s="7"/>
-      <c r="E146" s="15"/>
-      <c r="F146" s="7"/>
+      <c r="A146" s="6"/>
+      <c r="B146" s="6"/>
+      <c r="C146" s="6"/>
+      <c r="D146" s="6"/>
+      <c r="E146" s="12"/>
+      <c r="F146" s="6"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A147" s="7"/>
-      <c r="B147" s="7"/>
-      <c r="C147" s="7"/>
-      <c r="D147" s="7"/>
-      <c r="E147" s="15"/>
-      <c r="F147" s="7"/>
+      <c r="A147" s="6"/>
+      <c r="B147" s="6"/>
+      <c r="C147" s="6"/>
+      <c r="D147" s="6"/>
+      <c r="E147" s="12"/>
+      <c r="F147" s="6"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A148" s="7"/>
-      <c r="B148" s="7"/>
-      <c r="C148" s="7"/>
-      <c r="D148" s="7"/>
-      <c r="E148" s="15"/>
-      <c r="F148" s="7"/>
+      <c r="A148" s="6"/>
+      <c r="B148" s="6"/>
+      <c r="C148" s="6"/>
+      <c r="D148" s="6"/>
+      <c r="E148" s="12"/>
+      <c r="F148" s="6"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A149" s="7"/>
-      <c r="B149" s="7"/>
-      <c r="C149" s="7"/>
-      <c r="D149" s="7"/>
-      <c r="E149" s="15"/>
-      <c r="F149" s="7"/>
+      <c r="A149" s="6"/>
+      <c r="B149" s="6"/>
+      <c r="C149" s="6"/>
+      <c r="D149" s="6"/>
+      <c r="E149" s="12"/>
+      <c r="F149" s="6"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A150" s="7"/>
-      <c r="B150" s="7"/>
-      <c r="C150" s="7"/>
-      <c r="D150" s="7"/>
-      <c r="E150" s="15"/>
-      <c r="F150" s="7"/>
+      <c r="A150" s="6"/>
+      <c r="B150" s="6"/>
+      <c r="C150" s="6"/>
+      <c r="D150" s="6"/>
+      <c r="E150" s="12"/>
+      <c r="F150" s="6"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A151" s="7"/>
-      <c r="B151" s="7"/>
-      <c r="C151" s="7"/>
-      <c r="D151" s="7"/>
-      <c r="E151" s="15"/>
-      <c r="F151" s="7"/>
+      <c r="A151" s="6"/>
+      <c r="B151" s="6"/>
+      <c r="C151" s="6"/>
+      <c r="D151" s="6"/>
+      <c r="E151" s="12"/>
+      <c r="F151" s="6"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A152" s="7"/>
-      <c r="B152" s="7"/>
-      <c r="C152" s="7"/>
-      <c r="D152" s="7"/>
-      <c r="E152" s="15"/>
-      <c r="F152" s="7"/>
+      <c r="A152" s="6"/>
+      <c r="B152" s="6"/>
+      <c r="C152" s="6"/>
+      <c r="D152" s="6"/>
+      <c r="E152" s="12"/>
+      <c r="F152" s="6"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A153" s="7"/>
-      <c r="B153" s="7"/>
-      <c r="C153" s="7"/>
-      <c r="D153" s="7"/>
-      <c r="E153" s="15"/>
-      <c r="F153" s="7"/>
+      <c r="A153" s="6"/>
+      <c r="B153" s="6"/>
+      <c r="C153" s="6"/>
+      <c r="D153" s="6"/>
+      <c r="E153" s="12"/>
+      <c r="F153" s="6"/>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A154" s="7"/>
-      <c r="B154" s="7"/>
-      <c r="C154" s="7"/>
-      <c r="D154" s="7"/>
-      <c r="E154" s="15"/>
-      <c r="F154" s="7"/>
+      <c r="A154" s="6"/>
+      <c r="B154" s="6"/>
+      <c r="C154" s="6"/>
+      <c r="D154" s="6"/>
+      <c r="E154" s="12"/>
+      <c r="F154" s="6"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A155" s="7"/>
-      <c r="B155" s="7"/>
-      <c r="C155" s="7"/>
-      <c r="D155" s="7"/>
-      <c r="E155" s="15"/>
-      <c r="F155" s="7"/>
+      <c r="A155" s="6"/>
+      <c r="B155" s="6"/>
+      <c r="C155" s="6"/>
+      <c r="D155" s="6"/>
+      <c r="E155" s="12"/>
+      <c r="F155" s="6"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A156" s="7"/>
-      <c r="B156" s="7"/>
-      <c r="C156" s="7"/>
-      <c r="D156" s="7"/>
-      <c r="E156" s="15"/>
-      <c r="F156" s="7"/>
+      <c r="A156" s="6"/>
+      <c r="B156" s="6"/>
+      <c r="C156" s="6"/>
+      <c r="D156" s="6"/>
+      <c r="E156" s="12"/>
+      <c r="F156" s="6"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A157" s="7"/>
-      <c r="B157" s="7"/>
-      <c r="C157" s="7"/>
-      <c r="D157" s="7"/>
-      <c r="E157" s="15"/>
-      <c r="F157" s="7"/>
+      <c r="A157" s="6"/>
+      <c r="B157" s="6"/>
+      <c r="C157" s="6"/>
+      <c r="D157" s="6"/>
+      <c r="E157" s="12"/>
+      <c r="F157" s="6"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A158" s="7"/>
-      <c r="B158" s="7"/>
-      <c r="C158" s="7"/>
-      <c r="D158" s="7"/>
-      <c r="E158" s="15"/>
-      <c r="F158" s="7"/>
+      <c r="A158" s="6"/>
+      <c r="B158" s="6"/>
+      <c r="C158" s="6"/>
+      <c r="D158" s="6"/>
+      <c r="E158" s="12"/>
+      <c r="F158" s="6"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A159" s="7"/>
-      <c r="B159" s="7"/>
-      <c r="C159" s="7"/>
-      <c r="D159" s="7"/>
-      <c r="E159" s="15"/>
-      <c r="F159" s="7"/>
+      <c r="A159" s="6"/>
+      <c r="B159" s="6"/>
+      <c r="C159" s="6"/>
+      <c r="D159" s="6"/>
+      <c r="E159" s="12"/>
+      <c r="F159" s="6"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A160" s="7"/>
-      <c r="B160" s="7"/>
-      <c r="C160" s="7"/>
-      <c r="D160" s="7"/>
-      <c r="E160" s="15"/>
-      <c r="F160" s="7"/>
+      <c r="A160" s="6"/>
+      <c r="B160" s="6"/>
+      <c r="C160" s="6"/>
+      <c r="D160" s="6"/>
+      <c r="E160" s="12"/>
+      <c r="F160" s="6"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A161" s="7"/>
-      <c r="B161" s="7"/>
-      <c r="C161" s="7"/>
-      <c r="D161" s="7"/>
-      <c r="E161" s="15"/>
-      <c r="F161" s="7"/>
+      <c r="A161" s="6"/>
+      <c r="B161" s="6"/>
+      <c r="C161" s="6"/>
+      <c r="D161" s="6"/>
+      <c r="E161" s="12"/>
+      <c r="F161" s="6"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A162" s="7"/>
-      <c r="B162" s="7"/>
-      <c r="C162" s="7"/>
-      <c r="D162" s="7"/>
-      <c r="E162" s="15"/>
-      <c r="F162" s="7"/>
+      <c r="A162" s="6"/>
+      <c r="B162" s="6"/>
+      <c r="C162" s="6"/>
+      <c r="D162" s="6"/>
+      <c r="E162" s="12"/>
+      <c r="F162" s="6"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A163" s="7"/>
-      <c r="B163" s="7"/>
-      <c r="C163" s="7"/>
-      <c r="D163" s="7"/>
-      <c r="E163" s="15"/>
-      <c r="F163" s="7"/>
+      <c r="A163" s="6"/>
+      <c r="B163" s="6"/>
+      <c r="C163" s="6"/>
+      <c r="D163" s="6"/>
+      <c r="E163" s="12"/>
+      <c r="F163" s="6"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A164" s="7"/>
-      <c r="B164" s="7"/>
-      <c r="C164" s="7"/>
-      <c r="D164" s="7"/>
-      <c r="E164" s="15"/>
-      <c r="F164" s="7"/>
+      <c r="A164" s="6"/>
+      <c r="B164" s="6"/>
+      <c r="C164" s="6"/>
+      <c r="D164" s="6"/>
+      <c r="E164" s="12"/>
+      <c r="F164" s="6"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A165" s="7"/>
-      <c r="B165" s="7"/>
-      <c r="C165" s="7"/>
-      <c r="D165" s="7"/>
-      <c r="E165" s="15"/>
-      <c r="F165" s="7"/>
+      <c r="A165" s="6"/>
+      <c r="B165" s="6"/>
+      <c r="C165" s="6"/>
+      <c r="D165" s="6"/>
+      <c r="E165" s="12"/>
+      <c r="F165" s="6"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A166" s="7"/>
-      <c r="B166" s="7"/>
-      <c r="C166" s="7"/>
-      <c r="D166" s="7"/>
-      <c r="E166" s="15"/>
-      <c r="F166" s="7"/>
+      <c r="A166" s="6"/>
+      <c r="B166" s="6"/>
+      <c r="C166" s="6"/>
+      <c r="D166" s="6"/>
+      <c r="E166" s="12"/>
+      <c r="F166" s="6"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A167" s="7"/>
-      <c r="B167" s="7"/>
-      <c r="C167" s="7"/>
-      <c r="D167" s="7"/>
-      <c r="E167" s="15"/>
-      <c r="F167" s="7"/>
+      <c r="A167" s="6"/>
+      <c r="B167" s="6"/>
+      <c r="C167" s="6"/>
+      <c r="D167" s="6"/>
+      <c r="E167" s="12"/>
+      <c r="F167" s="6"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A168" s="7"/>
-      <c r="B168" s="7"/>
-      <c r="C168" s="7"/>
-      <c r="D168" s="7"/>
-      <c r="E168" s="15"/>
-      <c r="F168" s="7"/>
+      <c r="A168" s="6"/>
+      <c r="B168" s="6"/>
+      <c r="C168" s="6"/>
+      <c r="D168" s="6"/>
+      <c r="E168" s="12"/>
+      <c r="F168" s="6"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A169" s="7"/>
-      <c r="B169" s="7"/>
-      <c r="C169" s="7"/>
-      <c r="D169" s="7"/>
-      <c r="E169" s="15"/>
-      <c r="F169" s="7"/>
+      <c r="A169" s="6"/>
+      <c r="B169" s="6"/>
+      <c r="C169" s="6"/>
+      <c r="D169" s="6"/>
+      <c r="E169" s="12"/>
+      <c r="F169" s="6"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A170" s="7"/>
-      <c r="B170" s="7"/>
-      <c r="C170" s="7"/>
-      <c r="D170" s="7"/>
-      <c r="E170" s="15"/>
-      <c r="F170" s="7"/>
+      <c r="A170" s="6"/>
+      <c r="B170" s="6"/>
+      <c r="C170" s="6"/>
+      <c r="D170" s="6"/>
+      <c r="E170" s="12"/>
+      <c r="F170" s="6"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A171" s="7"/>
-      <c r="B171" s="7"/>
-      <c r="C171" s="7"/>
-      <c r="D171" s="7"/>
-      <c r="E171" s="15"/>
-      <c r="F171" s="7"/>
+      <c r="A171" s="6"/>
+      <c r="B171" s="6"/>
+      <c r="C171" s="6"/>
+      <c r="D171" s="6"/>
+      <c r="E171" s="12"/>
+      <c r="F171" s="6"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A172" s="7"/>
-      <c r="B172" s="7"/>
-      <c r="C172" s="7"/>
-      <c r="D172" s="7"/>
-      <c r="E172" s="15"/>
-      <c r="F172" s="7"/>
+      <c r="A172" s="6"/>
+      <c r="B172" s="6"/>
+      <c r="C172" s="6"/>
+      <c r="D172" s="6"/>
+      <c r="E172" s="12"/>
+      <c r="F172" s="6"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A173" s="7"/>
-      <c r="B173" s="7"/>
-      <c r="C173" s="7"/>
-      <c r="D173" s="7"/>
-      <c r="E173" s="15"/>
-      <c r="F173" s="7"/>
+      <c r="A173" s="6"/>
+      <c r="B173" s="6"/>
+      <c r="C173" s="6"/>
+      <c r="D173" s="6"/>
+      <c r="E173" s="12"/>
+      <c r="F173" s="6"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A174" s="7"/>
-      <c r="B174" s="7"/>
-      <c r="C174" s="7"/>
-      <c r="D174" s="7"/>
-      <c r="E174" s="15"/>
-      <c r="F174" s="7"/>
+      <c r="A174" s="6"/>
+      <c r="B174" s="6"/>
+      <c r="C174" s="6"/>
+      <c r="D174" s="6"/>
+      <c r="E174" s="12"/>
+      <c r="F174" s="6"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A175" s="7"/>
-      <c r="B175" s="7"/>
-      <c r="C175" s="7"/>
-      <c r="D175" s="7"/>
-      <c r="E175" s="15"/>
-      <c r="F175" s="7"/>
+      <c r="A175" s="6"/>
+      <c r="B175" s="6"/>
+      <c r="C175" s="6"/>
+      <c r="D175" s="6"/>
+      <c r="E175" s="12"/>
+      <c r="F175" s="6"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A176" s="7"/>
-      <c r="B176" s="7"/>
-      <c r="C176" s="7"/>
-      <c r="D176" s="7"/>
-      <c r="E176" s="15"/>
-      <c r="F176" s="7"/>
+      <c r="A176" s="6"/>
+      <c r="B176" s="6"/>
+      <c r="C176" s="6"/>
+      <c r="D176" s="6"/>
+      <c r="E176" s="12"/>
+      <c r="F176" s="6"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A177" s="7"/>
-      <c r="B177" s="7"/>
-      <c r="C177" s="7"/>
-      <c r="D177" s="7"/>
-      <c r="E177" s="15"/>
-      <c r="F177" s="7"/>
+      <c r="A177" s="6"/>
+      <c r="B177" s="6"/>
+      <c r="C177" s="6"/>
+      <c r="D177" s="6"/>
+      <c r="E177" s="12"/>
+      <c r="F177" s="6"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A178" s="7"/>
-      <c r="B178" s="7"/>
-      <c r="C178" s="7"/>
-      <c r="D178" s="7"/>
-      <c r="E178" s="15"/>
-      <c r="F178" s="7"/>
+      <c r="A178" s="6"/>
+      <c r="B178" s="6"/>
+      <c r="C178" s="6"/>
+      <c r="D178" s="6"/>
+      <c r="E178" s="12"/>
+      <c r="F178" s="6"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A179" s="7"/>
-      <c r="B179" s="7"/>
-      <c r="C179" s="7"/>
-      <c r="D179" s="7"/>
-      <c r="E179" s="15"/>
-      <c r="F179" s="7"/>
+      <c r="A179" s="6"/>
+      <c r="B179" s="6"/>
+      <c r="C179" s="6"/>
+      <c r="D179" s="6"/>
+      <c r="E179" s="12"/>
+      <c r="F179" s="6"/>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A180" s="7"/>
-      <c r="B180" s="7"/>
-      <c r="C180" s="7"/>
-      <c r="D180" s="7"/>
-      <c r="E180" s="15"/>
-      <c r="F180" s="7"/>
+      <c r="A180" s="6"/>
+      <c r="B180" s="6"/>
+      <c r="C180" s="6"/>
+      <c r="D180" s="6"/>
+      <c r="E180" s="12"/>
+      <c r="F180" s="6"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A181" s="7"/>
-      <c r="B181" s="7"/>
-      <c r="C181" s="7"/>
-      <c r="D181" s="7"/>
-      <c r="E181" s="15"/>
-      <c r="F181" s="7"/>
+      <c r="A181" s="6"/>
+      <c r="B181" s="6"/>
+      <c r="C181" s="6"/>
+      <c r="D181" s="6"/>
+      <c r="E181" s="12"/>
+      <c r="F181" s="6"/>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A182" s="7"/>
-      <c r="B182" s="7"/>
-      <c r="C182" s="7"/>
-      <c r="D182" s="7"/>
-      <c r="E182" s="15"/>
-      <c r="F182" s="7"/>
+      <c r="A182" s="6"/>
+      <c r="B182" s="6"/>
+      <c r="C182" s="6"/>
+      <c r="D182" s="6"/>
+      <c r="E182" s="12"/>
+      <c r="F182" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>